<commit_message>
Updating the missing files
</commit_message>
<xml_diff>
--- a/Data/DB_Detail.xlsx
+++ b/Data/DB_Detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jenkins\workspace\FFWF_QA_Automation\FFWF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EE307FBF-8B3B-46B6-9067-208F69C4F0A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E96BD3AF-E5DC-4BE5-97E5-481EFD69CC80}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="123">
   <si>
     <t>OrderNumber</t>
   </si>
@@ -261,9 +261,6 @@
   </si>
   <si>
     <t>ns2:FulfillmentReturnRequest/ns2:CustomerDetails/ns2:CustomerAccountIdentifier/Id</t>
-  </si>
-  <si>
-    <t>S110IPP064</t>
   </si>
   <si>
     <t>Resp_RequestId</t>
@@ -961,7 +958,7 @@
     </row>
     <row r="2" spans="1:10" ht="143.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>21</v>
@@ -973,7 +970,7 @@
         <v>83851</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -985,7 +982,7 @@
     </row>
     <row r="3" spans="1:10" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>22</v>
@@ -994,10 +991,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1009,7 +1006,7 @@
     </row>
     <row r="4" spans="1:10" ht="143.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>21</v>
@@ -1021,7 +1018,7 @@
         <v>83851</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1033,7 +1030,7 @@
     </row>
     <row r="5" spans="1:10" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>22</v>
@@ -1042,10 +1039,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1057,7 +1054,7 @@
     </row>
     <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>23</v>
@@ -1066,10 +1063,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="5">
-        <v>1944962</v>
+        <v>1957703</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -1081,7 +1078,7 @@
     </row>
     <row r="7" spans="1:10" ht="143.25" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>21</v>
@@ -1093,7 +1090,7 @@
         <v>83851</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1105,7 +1102,7 @@
     </row>
     <row r="8" spans="1:10" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>22</v>
@@ -1114,10 +1111,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1129,7 +1126,7 @@
     </row>
     <row r="9" spans="1:10" ht="143.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>21</v>
@@ -1141,7 +1138,7 @@
         <v>83851</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -1152,7 +1149,7 @@
     </row>
     <row r="10" spans="1:10" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>22</v>
@@ -1161,10 +1158,10 @@
         <v>7</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -1175,7 +1172,7 @@
     </row>
     <row r="11" spans="1:10" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>23</v>
@@ -1184,10 +1181,10 @@
         <v>8</v>
       </c>
       <c r="D11" s="5">
-        <v>1944962</v>
+        <v>1957703</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -1208,7 +1205,7 @@
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
@@ -1230,7 +1227,7 @@
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -1248,7 +1245,7 @@
       <c r="C14" s="18"/>
       <c r="D14" s="19"/>
       <c r="E14" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -1264,20 +1261,20 @@
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="G15" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="H15" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="I15" s="11" t="s">
         <v>24</v>
@@ -1292,20 +1289,20 @@
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="H16" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="I16" s="11" t="s">
         <v>25</v>
@@ -1320,20 +1317,20 @@
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="H17" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="I17" s="11" t="s">
         <v>26</v>
@@ -1352,16 +1349,16 @@
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="G18" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="H18" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="I18" s="11" t="s">
         <v>27</v>
@@ -1380,11 +1377,11 @@
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11" t="s">
@@ -1398,20 +1395,20 @@
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="G20" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="H20" s="13" t="s">
         <v>117</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>118</v>
       </c>
       <c r="I20" s="13" t="s">
         <v>32</v>
@@ -1426,20 +1423,20 @@
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="G21" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="H21" s="13" t="s">
         <v>117</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>118</v>
       </c>
       <c r="I21" s="13" t="s">
         <v>33</v>
@@ -1454,20 +1451,20 @@
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="G22" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="H22" s="13" t="s">
         <v>117</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>118</v>
       </c>
       <c r="I22" s="13" t="s">
         <v>34</v>
@@ -1486,16 +1483,16 @@
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="G23" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="H23" s="13" t="s">
         <v>117</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>118</v>
       </c>
       <c r="I23" s="13" t="s">
         <v>35</v>
@@ -1514,11 +1511,11 @@
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H24" s="13"/>
       <c r="I24" s="13" t="s">
@@ -1532,14 +1529,14 @@
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -1556,14 +1553,14 @@
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -1580,14 +1577,14 @@
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
@@ -1608,10 +1605,10 @@
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
@@ -1632,7 +1629,7 @@
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -1648,14 +1645,14 @@
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F30" s="13" t="s">
         <v>121</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>122</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
@@ -1672,14 +1669,14 @@
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="13" t="s">
         <v>121</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>122</v>
       </c>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
@@ -1696,14 +1693,14 @@
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="13" t="s">
         <v>121</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>122</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
@@ -1724,10 +1721,10 @@
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="13" t="s">
         <v>121</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>122</v>
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
@@ -1748,7 +1745,7 @@
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
@@ -1792,7 +1789,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="22"/>
     </row>
@@ -1801,17 +1798,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>92</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>93</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" t="s">
         <v>94</v>
-      </c>
-      <c r="F2" t="s">
-        <v>95</v>
       </c>
       <c r="G2">
         <v>14302428</v>
@@ -1822,20 +1819,20 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" t="s">
         <v>97</v>
-      </c>
-      <c r="G3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="63" x14ac:dyDescent="0.25">
@@ -1843,17 +1840,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G4">
         <v>14302428</v>
@@ -1864,20 +1861,20 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" t="s">
         <v>97</v>
-      </c>
-      <c r="G5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -1885,17 +1882,17 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G6">
         <v>11209031</v>

</xml_diff>